<commit_message>
Fix: Fix Error Exception and set Button Style
</commit_message>
<xml_diff>
--- a/data/상훈모의고사/상훈모의고사 학생 제출 답.xlsx
+++ b/data/상훈모의고사/상훈모의고사 학생 제출 답.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/isanghun/grade_analysis/data/상훈모의고사/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353B8246-57F0-364D-ACBF-3874AC77CC95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47FA382F-F28D-6D4A-934B-5139A7DDBBAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1220" yWindow="3000" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2200" yWindow="5020" windowWidth="25600" windowHeight="16000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>분당</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>11111222223333344441</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -53,6 +49,10 @@
   </si>
   <si>
     <t>11111222223333344433</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>서현</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -417,7 +417,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -441,21 +441,21 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>